<commit_message>
fixing key problems in crypto
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_2288.xlsx
+++ b/bioSample/bioSample_2288.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">replicate</t>
   </si>
   <si>
-    <t xml:space="preserve">5.16.17</t>
+    <t xml:space="preserve">05.16.17</t>
   </si>
   <si>
     <t xml:space="preserve">H.BROWN</t>
@@ -194,13 +194,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -223,7 +227,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -260,7 +264,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>9</v>
       </c>
@@ -289,8 +293,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -318,8 +322,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
@@ -347,8 +351,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="0" t="s">
@@ -376,8 +380,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="0" t="s">
@@ -405,8 +409,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="0" t="s">
@@ -434,8 +438,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="0" t="s">
@@ -463,8 +467,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="0" t="s">
@@ -492,8 +496,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
@@ -521,8 +525,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
@@ -550,8 +554,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="0" t="s">
@@ -579,8 +583,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="0" t="s">
@@ -608,8 +612,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="0" t="s">
@@ -634,8 +638,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="0" t="s">
@@ -660,8 +664,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="0" t="s">
@@ -686,8 +690,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="0" t="s">
@@ -715,8 +719,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="0" t="s">
@@ -744,8 +748,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="0" t="s">
@@ -773,8 +777,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="0" t="s">
@@ -802,8 +806,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B21" s="0" t="s">
@@ -831,8 +835,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B22" s="0" t="s">
@@ -860,8 +864,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B23" s="0" t="s">
@@ -889,8 +893,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B24" s="0" t="s">
@@ -918,8 +922,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B25" s="0" t="s">

</xml_diff>